<commit_message>
Fix bug for duplicate shopify orders during update. Work on update function not keeping old shopee names
</commit_message>
<xml_diff>
--- a/Product Setting.xlsx
+++ b/Product Setting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaiwei\Desktop\TKG Inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30EDC5A1-D4C5-47A8-9F2E-DA2E7C0AE709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1ED657E-1A62-45D1-ACA3-19A964EADA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{3AAD4353-909F-49E8-AF1D-E8E318291889}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{669A9A0F-AF93-45D6-8026-8EB8742234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -838,7 +838,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC20637-F7DF-418D-9764-89AB51F7F39A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3275A25D-B5AB-4845-A103-BE69CECDF794}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA127"/>
   <sheetViews>

</xml_diff>